<commit_message>
changes to mlx_cam calculations
changed the center of the camera for calculations
</commit_message>
<xml_diff>
--- a/ME_405 Calculations.xlsx
+++ b/ME_405 Calculations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cpslo-my.sharepoint.com/personal/muldrow_calpoly_edu/Documents/Documents/1.0 FILES FOR COLLEGE/6.0 Winter 2024/ME-405 LAB/Term Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{39F78E74-28BC-4D09-9F3A-4C0FC442C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{116BF26B-380E-452E-9651-B193BDE7CDFD}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{39F78E74-28BC-4D09-9F3A-4C0FC442C6C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{81276033-FE31-4570-AF41-8C5258EB9780}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E51D0BAD-58B1-4399-81A7-FDA2ECB91A9C}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="59">
   <si>
     <t>Values</t>
   </si>
@@ -274,6 +274,30 @@
   </si>
   <si>
     <t>exp columns (calc'd)</t>
+  </si>
+  <si>
+    <t>Turret 180</t>
+  </si>
+  <si>
+    <t>Column Calculator</t>
+  </si>
+  <si>
+    <t>column</t>
+  </si>
+  <si>
+    <t>negative (&lt;15)</t>
+  </si>
+  <si>
+    <t>tics (&gt;15)</t>
+  </si>
+  <si>
+    <t>exp tics (calc'd)</t>
+  </si>
+  <si>
+    <t>Expected Angle</t>
+  </si>
+  <si>
+    <t>pos angle</t>
   </si>
 </sst>
 </file>
@@ -354,7 +378,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -517,11 +541,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -552,6 +600,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -886,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A37494B7-BBEC-48D8-9C60-CEBD98A19F56}">
-  <dimension ref="B3:Z26"/>
+  <dimension ref="B3:Z34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.109375" defaultRowHeight="16.8" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -920,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="D4" s="4">
-        <v>6600</v>
+        <v>3280</v>
       </c>
       <c r="E4" t="s">
         <v>5</v>
@@ -941,7 +994,7 @@
         <v>47</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="O4" s="13" t="s">
         <v>48</v>
@@ -985,7 +1038,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="4">
-        <v>180</v>
+        <v>90</v>
       </c>
       <c r="E5" t="s">
         <v>6</v>
@@ -997,17 +1050,17 @@
         <v>1</v>
       </c>
       <c r="K5" s="14">
-        <f>ATAN(I5/$D$14)*(180/PI())</f>
+        <f>ATAN(I5/$D$15)*(180/PI())</f>
         <v>1.9091524329963763</v>
       </c>
       <c r="L5" s="16"/>
       <c r="M5" s="14">
-        <f>K5*$D$6</f>
-        <v>70.002255876533795</v>
+        <f>K5*$D$7</f>
+        <v>69.577999780312382</v>
       </c>
       <c r="N5" s="16"/>
       <c r="O5" s="14">
-        <f>K5*(1/$D$10)</f>
+        <f>K5*(1/$D$11)</f>
         <v>1.1107795973797099</v>
       </c>
       <c r="P5" s="16"/>
@@ -1024,67 +1077,61 @@
     </row>
     <row r="6" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="4">
+        <f>(180/D5)*D4</f>
+        <v>6560</v>
+      </c>
+      <c r="I6" s="24"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+    </row>
+    <row r="7" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="4">
-        <f>6600/180</f>
-        <v>36.666666666666664</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="D7" s="4">
+        <f>D6/180</f>
+        <v>36.444444444444443</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="20">
+      <c r="I7" s="20">
         <v>0.5</v>
       </c>
-      <c r="J6" s="18">
+      <c r="J7" s="18">
         <v>2</v>
       </c>
-      <c r="K6" s="14">
-        <f t="shared" ref="K6:K18" si="0">ATAN(I6/$D$14)*(180/PI())</f>
+      <c r="K7" s="14">
+        <f t="shared" ref="K7:K19" si="0">ATAN(I7/$D$15)*(180/PI())</f>
         <v>1.9091524329963763</v>
-      </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="14">
-        <f t="shared" ref="M6:M18" si="1">K6*$D$6</f>
-        <v>70.002255876533795</v>
-      </c>
-      <c r="N6" s="16"/>
-      <c r="O6" s="14">
-        <f t="shared" ref="O6:O18" si="2">K6*(1/$D$10)</f>
-        <v>1.1107795973797099</v>
-      </c>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-    </row>
-    <row r="7" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I7" s="20">
-        <v>-0.5</v>
-      </c>
-      <c r="J7" s="18">
-        <v>1</v>
-      </c>
-      <c r="K7" s="14">
-        <f t="shared" si="0"/>
-        <v>-1.9091524329963763</v>
       </c>
       <c r="L7" s="16"/>
       <c r="M7" s="14">
-        <f t="shared" si="1"/>
-        <v>-70.002255876533795</v>
+        <f t="shared" ref="M7:M19" si="1">K7*$D$7</f>
+        <v>69.577999780312382</v>
       </c>
       <c r="N7" s="16"/>
       <c r="O7" s="14">
-        <f t="shared" si="2"/>
-        <v>-1.1107795973797099</v>
+        <f t="shared" ref="O7:O19" si="2">K7*(1/$D$11)</f>
+        <v>1.1107795973797099</v>
       </c>
       <c r="P7" s="16"/>
       <c r="Q7" s="23"/>
@@ -1099,23 +1146,11 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4">
-        <v>55</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4</v>
-      </c>
       <c r="I8" s="20">
         <v>-0.5</v>
       </c>
       <c r="J8" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K8" s="14">
         <f t="shared" si="0"/>
@@ -1124,7 +1159,7 @@
       <c r="L8" s="16"/>
       <c r="M8" s="14">
         <f t="shared" si="1"/>
-        <v>-70.002255876533795</v>
+        <v>-69.577999780312382</v>
       </c>
       <c r="N8" s="16"/>
       <c r="O8" s="14">
@@ -1144,34 +1179,37 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="5" t="s">
+        <v>7</v>
+      </c>
       <c r="C9" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D9" s="4">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I9" s="20">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="J9" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-1.9091524329963763</v>
       </c>
       <c r="L9" s="16"/>
       <c r="M9" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>-69.577999780312382</v>
       </c>
       <c r="N9" s="16"/>
       <c r="O9" s="14">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1.1107795973797099</v>
       </c>
       <c r="P9" s="16"/>
       <c r="Q9" s="23"/>
@@ -1187,20 +1225,19 @@
     </row>
     <row r="10" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" s="4">
-        <f>D8/D9</f>
-        <v>1.71875</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I10" s="20">
         <v>0</v>
       </c>
       <c r="J10" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="14">
         <f t="shared" si="0"/>
@@ -1230,34 +1267,34 @@
     </row>
     <row r="11" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D11" s="4">
-        <f>D6*D10</f>
-        <v>63.020833333333329</v>
+        <f>D9/D10</f>
+        <v>1.71875</v>
       </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I11" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="14">
         <f t="shared" si="0"/>
-        <v>3.8140748342903543</v>
+        <v>0</v>
       </c>
       <c r="L11" s="16"/>
       <c r="M11" s="14">
         <f t="shared" si="1"/>
-        <v>139.84941059064633</v>
+        <v>0</v>
       </c>
       <c r="N11" s="16"/>
       <c r="O11" s="14">
         <f t="shared" si="2"/>
-        <v>2.2190980854052968</v>
+        <v>0</v>
       </c>
       <c r="P11" s="16"/>
       <c r="Q11" s="23"/>
@@ -1272,11 +1309,21 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4">
+        <f>D7*D11</f>
+        <v>62.638888888888886</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
       <c r="I12" s="20">
         <v>1</v>
       </c>
       <c r="J12" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K12" s="14">
         <f t="shared" si="0"/>
@@ -1285,7 +1332,7 @@
       <c r="L12" s="16"/>
       <c r="M12" s="14">
         <f t="shared" si="1"/>
-        <v>139.84941059064633</v>
+        <v>139.00183840524846</v>
       </c>
       <c r="N12" s="16"/>
       <c r="O12" s="14">
@@ -1305,37 +1352,25 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" t="s">
-        <v>20</v>
-      </c>
       <c r="I13" s="20">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="J13" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="14">
         <f t="shared" si="0"/>
-        <v>-3.8140748342903543</v>
+        <v>3.8140748342903543</v>
       </c>
       <c r="L13" s="16"/>
       <c r="M13" s="14">
         <f t="shared" si="1"/>
-        <v>-139.84941059064633</v>
+        <v>139.00183840524846</v>
       </c>
       <c r="N13" s="16"/>
       <c r="O13" s="14">
         <f t="shared" si="2"/>
-        <v>-2.2190980854052968</v>
+        <v>2.2190980854052968</v>
       </c>
       <c r="P13" s="16"/>
       <c r="Q13" s="23"/>
@@ -1349,12 +1384,15 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="2:26" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="3" t="s">
-        <v>21</v>
+    <row r="14" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>19</v>
       </c>
       <c r="D14" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
         <v>20</v>
@@ -1363,7 +1401,7 @@
         <v>-1</v>
       </c>
       <c r="J14" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K14" s="14">
         <f t="shared" si="0"/>
@@ -1372,7 +1410,7 @@
       <c r="L14" s="16"/>
       <c r="M14" s="14">
         <f t="shared" si="1"/>
-        <v>-139.84941059064633</v>
+        <v>-139.00183840524846</v>
       </c>
       <c r="N14" s="16"/>
       <c r="O14" s="14">
@@ -1391,36 +1429,35 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="2" t="s">
-        <v>22</v>
+    <row r="15" spans="2:26" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D15" s="2">
-        <f>ATAN((D13/2)/D14)*(180/PI())</f>
-        <v>9.4623222080256166</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="I15" s="20">
+        <v>-1</v>
+      </c>
+      <c r="J15" s="18">
         <v>2</v>
-      </c>
-      <c r="J15" s="18">
-        <v>1</v>
       </c>
       <c r="K15" s="14">
         <f t="shared" si="0"/>
-        <v>7.594643368591445</v>
+        <v>-3.8140748342903543</v>
       </c>
       <c r="L15" s="16"/>
       <c r="M15" s="14">
         <f t="shared" si="1"/>
-        <v>278.47025684835296</v>
+        <v>-139.00183840524846</v>
       </c>
       <c r="N15" s="16"/>
       <c r="O15" s="14">
         <f t="shared" si="2"/>
-        <v>4.4187015962713856</v>
+        <v>-2.2190980854052968</v>
       </c>
       <c r="P15" s="16"/>
       <c r="Q15" s="23"/>
@@ -1436,20 +1473,20 @@
     </row>
     <row r="16" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="2">
-        <f>D15*(1/D10)</f>
-        <v>5.5053511028512672</v>
+        <f>ATAN((D14/2)/D15)*(180/PI())</f>
+        <v>7.594643368591445</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I16" s="20">
         <v>2</v>
       </c>
       <c r="J16" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K16" s="14">
         <f t="shared" si="0"/>
@@ -1458,7 +1495,7 @@
       <c r="L16" s="16"/>
       <c r="M16" s="14">
         <f t="shared" si="1"/>
-        <v>278.47025684835296</v>
+        <v>276.78255832199932</v>
       </c>
       <c r="N16" s="16"/>
       <c r="O16" s="14">
@@ -1479,34 +1516,34 @@
     </row>
     <row r="17" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D17" s="2">
-        <f>D11*D16</f>
-        <v>346.95181429427254</v>
+        <f>D16*(1/D11)</f>
+        <v>4.4187015962713856</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I17" s="20">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="J17" s="18">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="14">
         <f t="shared" si="0"/>
-        <v>-7.594643368591445</v>
+        <v>7.594643368591445</v>
       </c>
       <c r="L17" s="16"/>
       <c r="M17" s="14">
         <f t="shared" si="1"/>
-        <v>-278.47025684835296</v>
+        <v>276.78255832199932</v>
       </c>
       <c r="N17" s="16"/>
       <c r="O17" s="14">
         <f t="shared" si="2"/>
-        <v>-4.4187015962713856</v>
+        <v>4.4187015962713856</v>
       </c>
       <c r="P17" s="16"/>
       <c r="Q17" s="23"/>
@@ -1520,26 +1557,36 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="2:26" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I18" s="21">
-        <v>2</v>
+    <row r="18" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="2">
+        <f>D12*D17</f>
+        <v>276.78255832199926</v>
+      </c>
+      <c r="E18" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="20">
+        <v>-2</v>
       </c>
       <c r="J18" s="18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K18" s="14">
         <f t="shared" si="0"/>
-        <v>7.594643368591445</v>
+        <v>-7.594643368591445</v>
       </c>
       <c r="L18" s="16"/>
       <c r="M18" s="14">
         <f t="shared" si="1"/>
-        <v>278.47025684835296</v>
+        <v>-276.78255832199932</v>
       </c>
       <c r="N18" s="16"/>
       <c r="O18" s="14">
         <f t="shared" si="2"/>
-        <v>4.4187015962713856</v>
+        <v>-4.4187015962713856</v>
       </c>
       <c r="P18" s="16"/>
       <c r="Q18" s="23"/>
@@ -1553,85 +1600,179 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="2:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="6" t="s">
+    <row r="19" spans="2:26" ht="16.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="21">
+        <v>2</v>
+      </c>
+      <c r="J19" s="18">
+        <v>2</v>
+      </c>
+      <c r="K19" s="14">
+        <f t="shared" si="0"/>
+        <v>7.594643368591445</v>
+      </c>
+      <c r="L19" s="16"/>
+      <c r="M19" s="14">
+        <f t="shared" si="1"/>
+        <v>276.78255832199932</v>
+      </c>
+      <c r="N19" s="16"/>
+      <c r="O19" s="14">
+        <f t="shared" si="2"/>
+        <v>4.4187015962713856</v>
+      </c>
+      <c r="P19" s="16"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="2"/>
+      <c r="V19" s="2"/>
+      <c r="W19" s="2"/>
+      <c r="X19" s="2"/>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="2"/>
+    </row>
+    <row r="20" spans="2:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D20" s="9">
         <v>1</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E20" t="s">
         <v>20</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="2:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="7" t="s">
+    <row r="21" spans="2:26" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="8">
-        <f>ATAN(D19/D14)*(180/PI())</f>
+      <c r="D21" s="8">
+        <f>ATAN(D20/D15)*(180/PI())</f>
         <v>3.8140748342903543</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E21" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="8">
-        <f>D20*D6</f>
-        <v>139.84941059064633</v>
-      </c>
-      <c r="E21" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="8">
+        <f>D21*D7</f>
+        <v>139.00183840524846</v>
+      </c>
+      <c r="E22" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D22" s="8">
-        <f>D20*(1/D10)</f>
+      <c r="D23" s="8">
+        <f>D21*(1/D11)</f>
         <v>2.2190980854052968</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="23" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="F23" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="24" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="5" t="s">
-        <v>31</v>
-      </c>
+      <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C25" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="8">
-        <f>15.5-D22</f>
-        <v>13.280901914594704</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C26" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="8">
+        <f>15.5-D23</f>
+        <v>13.280901914594704</v>
+      </c>
+    </row>
+    <row r="27" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D26" s="8">
-        <f>15.5+D22</f>
+      <c r="D27" s="8">
+        <f>15.5+D23</f>
         <v>17.719098085405296</v>
+      </c>
+    </row>
+    <row r="29" spans="2:26" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="5">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="2:26" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="25"/>
+      <c r="C30" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D30" s="5">
+        <f>(-15.5+D29)*D11</f>
+        <v>6.015625</v>
+      </c>
+    </row>
+    <row r="31" spans="2:26" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="25"/>
+      <c r="C31" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" s="5">
+        <f>(-15.5+D29)*D12</f>
+        <v>219.23611111111109</v>
+      </c>
+    </row>
+    <row r="32" spans="2:26" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C32" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" s="5">
+        <f>(15.5-D29)*-D12</f>
+        <v>219.23611111111109</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="5">
+        <f>D31*(1/D7)</f>
+        <v>6.0156249999999991</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C34" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34">
+        <f>D32*(1/D7)</f>
+        <v>6.0156249999999991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>